<commit_message>
reading from excel file and testing api finished
</commit_message>
<xml_diff>
--- a/src/test/resources/loginTestCases.xlsx
+++ b/src/test/resources/loginTestCases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>cagvq34v@</t>
+  </si>
+  <si>
+    <t>""</t>
   </si>
 </sst>
 </file>
@@ -865,7 +868,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,6 +954,9 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
       <c r="D5">
         <v>401</v>
       </c>
@@ -962,6 +968,9 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -976,6 +985,12 @@
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
       <c r="D7">
         <v>401</v>
       </c>
@@ -1007,9 +1022,6 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
       <c r="D9">
         <v>401</v>
       </c>
@@ -1021,9 +1033,6 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
@@ -1037,12 +1046,6 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
       </c>
       <c r="D11">
         <v>401</v>

</xml_diff>

<commit_message>
expecting 500, but should never do that
</commit_message>
<xml_diff>
--- a/src/test/resources/loginTestCases.xlsx
+++ b/src/test/resources/loginTestCases.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="loginTestCases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -58,13 +58,25 @@
   </si>
   <si>
     <t>""</t>
+  </si>
+  <si>
+    <t>teacher_abai_school</t>
+  </si>
+  <si>
+    <t>=pkFg4tf60AW</t>
+  </si>
+  <si>
+    <t>Internal Server Error</t>
+  </si>
+  <si>
+    <t>Internal Server Error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +210,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0451A5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -541,9 +559,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -865,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,10 +1059,10 @@
         <v>6</v>
       </c>
       <c r="D10">
-        <v>401</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
+        <v>500</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1048,10 +1070,24 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>401</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
+        <v>500</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>